<commit_message>
I made Test2 have rough breaking numbers with Dx as a variable instead of setting the maximum possible like in the paper
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william_hess/Desktop/FSAE/Local_Copy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william_hess/Desktop/FSAE/taiyangie-LinkageForceAnalyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74DE3102-1514-7446-AD53-ED06A8E4F0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FBA68F-4C9A-004D-B155-02CCBA9C6B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17100" yWindow="500" windowWidth="16500" windowHeight="17440" xr2:uid="{BAE74CFE-6EF5-2142-B21E-1769416C9AE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -107,13 +107,19 @@
     <t>#</t>
   </si>
   <si>
-    <t>G forces</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
     <t>Gs</t>
+  </si>
+  <si>
+    <t>Gs of Acceleration</t>
+  </si>
+  <si>
+    <t>Gs of Deceleration</t>
+  </si>
+  <si>
+    <t>Dx</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65311B17-CA08-AF4C-B517-392D7033E157}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,13 +583,24 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to do Steady State with no Luck
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william_hess/Desktop/FSAE/taiyangie-LinkageForceAnalyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FBA68F-4C9A-004D-B155-02CCBA9C6B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D232C58-3D68-7741-867B-245207490E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17100" yWindow="500" windowWidth="16500" windowHeight="17440" xr2:uid="{BAE74CFE-6EF5-2142-B21E-1769416C9AE4}"/>
+    <workbookView xWindow="19080" yWindow="500" windowWidth="14520" windowHeight="17440" xr2:uid="{BAE74CFE-6EF5-2142-B21E-1769416C9AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
@@ -84,18 +84,6 @@
   </si>
   <si>
     <t>r</t>
-  </si>
-  <si>
-    <t>Center of Gravity to Rear Axle</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Center of Gravity to Front Axle</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
   <si>
     <t>mu</t>
@@ -471,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65311B17-CA08-AF4C-B517-392D7033E157}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,13 +516,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -561,46 +549,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>